<commit_message>
Seznam materialu pro Standu.
</commit_message>
<xml_diff>
--- a/Designs/Spectrograph/doc/src/material_bill.xlsx
+++ b/Designs/Spectrograph/doc/src/material_bill.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>TRIACSHARP02A</t>
   </si>
@@ -42,9 +42,6 @@
     <t>DS18B20</t>
   </si>
   <si>
-    <t>ratky cerny</t>
-  </si>
-  <si>
     <t>kratky cerveny</t>
   </si>
   <si>
@@ -72,19 +69,28 @@
     <t>dlouhy zluty</t>
   </si>
   <si>
-    <t>3 plast</t>
-  </si>
-  <si>
-    <t>4 plast</t>
-  </si>
-  <si>
-    <t>5 plast</t>
-  </si>
-  <si>
     <t xml:space="preserve">faston </t>
   </si>
   <si>
     <t>valcovy konektor</t>
+  </si>
+  <si>
+    <t>BASE162101A</t>
+  </si>
+  <si>
+    <t>3 plast dutinka</t>
+  </si>
+  <si>
+    <t>4 plast dutinka</t>
+  </si>
+  <si>
+    <t>5 plast dutinka</t>
+  </si>
+  <si>
+    <t>1 plast dutinka</t>
+  </si>
+  <si>
+    <t>kratky cerny</t>
   </si>
 </sst>
 </file>
@@ -424,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,7 +502,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -504,7 +510,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -512,7 +518,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>5</v>
@@ -520,7 +526,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -528,7 +534,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>7</v>
@@ -536,7 +542,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -544,7 +550,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -552,7 +558,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -560,57 +566,107 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
       <c r="B17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <f>SUM(B8:B17)</f>
+        <v>37</v>
+      </c>
+      <c r="D17">
+        <f>C17*2</f>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <f>C18*B18</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ref="D19:D20" si="0">C19*B19</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E20">
+        <f>SUM(D18:D20)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B21">
+        <f>D17-E20</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24">
         <v>1</v>
       </c>
     </row>

</xml_diff>